<commit_message>
converting URIs into w3id.org/italia/controlled-vocabulary for authentication-type controlled vocabulary and inserted German translations; uploaded a presentation in ITA on DAF+OpenData
</commit_message>
<xml_diff>
--- a/VocabolariControllati/classifications-for-public-services/authentication-type/authentication-type.xlsx
+++ b/VocabolariControllati/classifications-for-public-services/authentication-type/authentication-type.xlsx
@@ -19,44 +19,23 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="38" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="60">
   <si>
     <t>Autenticazione singolo fattore</t>
   </si>
   <si>
-    <t>UserId &amp; Password (PIN, NoiPA, FiscoOnline e ogni altro sistema che richiede solo credenziali di tipo usernid e pwd)</t>
-  </si>
-  <si>
     <t>SPIDL1</t>
   </si>
   <si>
-    <t>Autenticazione doppio fattore</t>
-  </si>
-  <si>
     <t>SPIDL2</t>
   </si>
   <si>
-    <t>Autenticazione doppio fattore hardware</t>
-  </si>
-  <si>
     <t>CIE</t>
   </si>
   <si>
-    <t>Codice 1 Livello</t>
-  </si>
-  <si>
-    <t>Label 1 Livello</t>
-  </si>
-  <si>
     <t>NONE</t>
   </si>
   <si>
-    <t>Codice 2 Livello</t>
-  </si>
-  <si>
-    <t>Label 2 Livello</t>
-  </si>
-  <si>
     <t>SFA</t>
   </si>
   <si>
@@ -90,9 +69,6 @@
     <t>SPID Livello 3</t>
   </si>
   <si>
-    <t>Carta nazionale dei servizi (CNS) (include anche Tessera Sanitaria-CNS)</t>
-  </si>
-  <si>
     <t>CNS</t>
   </si>
   <si>
@@ -109,6 +85,120 @@
   </si>
   <si>
     <t>User ID, One Time Password e Biometria</t>
+  </si>
+  <si>
+    <t>None - free access</t>
+  </si>
+  <si>
+    <t>Keine - freier Zugang</t>
+  </si>
+  <si>
+    <t>Single Factor Authentication</t>
+  </si>
+  <si>
+    <t>Single-Faktor-Authentifizierung</t>
+  </si>
+  <si>
+    <t>User ID e Password</t>
+  </si>
+  <si>
+    <t>User ID and password</t>
+  </si>
+  <si>
+    <t>Benutzer-ID und Passwort</t>
+  </si>
+  <si>
+    <t>SPID (National public system of e-ID) Credential Level 1</t>
+  </si>
+  <si>
+    <t>SPID (Nationales öffentliches System der e-ID) Berechtigungsnachweis Stufe 1</t>
+  </si>
+  <si>
+    <t>Autenticazione a due fattori</t>
+  </si>
+  <si>
+    <t>Two Factor Authentication</t>
+  </si>
+  <si>
+    <t>Zwei-Faktor-Authentifizierung</t>
+  </si>
+  <si>
+    <t>User ID and One Time Password</t>
+  </si>
+  <si>
+    <t>Benutzer-ID und Einmal-Passwort</t>
+  </si>
+  <si>
+    <t>SPID (National public system of e-ID) Level 2</t>
+  </si>
+  <si>
+    <t>SPID (Nationales öffentliches System der e-ID) Stufe 2</t>
+  </si>
+  <si>
+    <t>Autenticazione a due fattori hardware</t>
+  </si>
+  <si>
+    <t>Two Factor Authentication hardware</t>
+  </si>
+  <si>
+    <t>Zwei-Faktor-Hardware-Authentifizierung</t>
+  </si>
+  <si>
+    <t>SPID (National public system of e-ID) Level 3</t>
+  </si>
+  <si>
+    <t>SPID (Nationales öffentliches System der e-ID) Stufe 3</t>
+  </si>
+  <si>
+    <t>Carta nazionale dei servizi (CNS)</t>
+  </si>
+  <si>
+    <t>National service card</t>
+  </si>
+  <si>
+    <t>Nationale Servicekarte</t>
+  </si>
+  <si>
+    <t>Electronic identity card</t>
+  </si>
+  <si>
+    <t>Elektronischer Personalausweis (CIE)</t>
+  </si>
+  <si>
+    <t>Multi-factor authentication</t>
+  </si>
+  <si>
+    <t>Multi-Faktor-Authentifizierung</t>
+  </si>
+  <si>
+    <t>User ID, One Time Password and Biometric</t>
+  </si>
+  <si>
+    <t>Benutzer-ID, Einmalpasswort und biometrische Daten</t>
+  </si>
+  <si>
+    <t>codice_1_livello</t>
+  </si>
+  <si>
+    <t>label_ITA_1_livello</t>
+  </si>
+  <si>
+    <t>label_ENG_1_livello</t>
+  </si>
+  <si>
+    <t>label_DEU_1_livello</t>
+  </si>
+  <si>
+    <t>codice_2_livello</t>
+  </si>
+  <si>
+    <t>label_ITA_2_livello</t>
+  </si>
+  <si>
+    <t>label_ENG_2_livello</t>
+  </si>
+  <si>
+    <t>label_DEU_2_livello</t>
   </si>
 </sst>
 </file>
@@ -121,6 +211,7 @@
       <color theme="1"/>
       <name val="Calibri"/>
       <family val="2"/>
+      <charset val="136"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -187,7 +278,7 @@
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
@@ -199,6 +290,9 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="13">
@@ -543,10 +637,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D10"/>
+  <dimension ref="A1:H10"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C30" sqref="C30"/>
+    <sheetView tabSelected="1" zoomScale="150" zoomScaleNormal="150" zoomScalePageLayoutView="150" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0"/>
@@ -555,141 +649,259 @@
     <col min="2" max="2" width="34.33203125" customWidth="1"/>
     <col min="3" max="3" width="45.33203125" customWidth="1"/>
     <col min="4" max="4" width="59.5" customWidth="1"/>
+    <col min="5" max="5" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="39.83203125" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="44.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="22.6640625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:8">
       <c r="A1" s="3" t="s">
-        <v>7</v>
+        <v>52</v>
       </c>
       <c r="B1" s="3" t="s">
-        <v>8</v>
+        <v>53</v>
       </c>
       <c r="C1" s="3" t="s">
-        <v>10</v>
+        <v>54</v>
       </c>
       <c r="D1" s="3" t="s">
-        <v>11</v>
+        <v>55</v>
+      </c>
+      <c r="E1" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="F1" s="3" t="s">
+        <v>57</v>
+      </c>
+      <c r="G1" s="3" t="s">
+        <v>58</v>
+      </c>
+      <c r="H1" s="3" t="s">
+        <v>59</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:8">
       <c r="A2" t="s">
-        <v>9</v>
+        <v>4</v>
       </c>
       <c r="B2" s="5" t="s">
-        <v>13</v>
-      </c>
-      <c r="C2" s="1"/>
+        <v>6</v>
+      </c>
+      <c r="C2" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="D2" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="E2" s="1"/>
     </row>
-    <row r="3" spans="1:4" ht="30">
+    <row r="3" spans="1:8">
       <c r="A3" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B3" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C3" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3" s="2" t="s">
-        <v>1</v>
+      <c r="C3" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E3" s="4" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="G3" t="s">
+        <v>27</v>
+      </c>
+      <c r="H3" t="s">
+        <v>28</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:8" ht="75">
       <c r="A4" s="4" t="s">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="B4" s="5" t="s">
         <v>0</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="D4" s="5" t="s">
+        <v>25</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="G4" s="6" t="s">
+        <v>29</v>
+      </c>
+      <c r="H4" s="6" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8">
+      <c r="A5" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C5" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D5" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E5" t="s">
+        <v>11</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="G5" t="s">
+        <v>34</v>
+      </c>
+      <c r="H5" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8">
+      <c r="A6" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C6" s="5" t="s">
+        <v>32</v>
+      </c>
+      <c r="D6" s="5" t="s">
+        <v>33</v>
+      </c>
+      <c r="E6" t="s">
         <v>2</v>
       </c>
-      <c r="D4" s="1" t="s">
+      <c r="F6" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="G6" t="s">
+        <v>36</v>
+      </c>
+      <c r="H6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8">
+      <c r="A7" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C7" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D7" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E7" t="s">
+        <v>14</v>
+      </c>
+      <c r="F7" s="1" t="s">
         <v>15</v>
       </c>
+      <c r="G7" t="s">
+        <v>41</v>
+      </c>
+      <c r="H7" t="s">
+        <v>42</v>
+      </c>
     </row>
-    <row r="5" spans="1:4">
-      <c r="A5" t="s">
+    <row r="8" spans="1:8">
+      <c r="A8" t="s">
+        <v>13</v>
+      </c>
+      <c r="B8" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C8" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D8" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E8" t="s">
         <v>16</v>
       </c>
-      <c r="B5" s="5" t="s">
+      <c r="F8" s="1" t="s">
+        <v>43</v>
+      </c>
+      <c r="G8" t="s">
+        <v>44</v>
+      </c>
+      <c r="H8" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8">
+      <c r="A9" t="s">
+        <v>13</v>
+      </c>
+      <c r="B9" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C9" s="5" t="s">
+        <v>39</v>
+      </c>
+      <c r="D9" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E9" t="s">
         <v>3</v>
       </c>
-      <c r="C5" t="s">
+      <c r="F9" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="G9" t="s">
+        <v>46</v>
+      </c>
+      <c r="H9" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8">
+      <c r="A10" t="s">
         <v>18</v>
       </c>
-      <c r="D5" s="1" t="s">
+      <c r="B10" s="5" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="6" spans="1:4">
-      <c r="A6" t="s">
-        <v>16</v>
-      </c>
-      <c r="B6" s="5" t="s">
-        <v>3</v>
-      </c>
-      <c r="C6" t="s">
-        <v>4</v>
-      </c>
-      <c r="D6" s="1" t="s">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4">
-      <c r="A7" t="s">
+      <c r="C10" s="5" t="s">
+        <v>48</v>
+      </c>
+      <c r="D10" s="5" t="s">
+        <v>49</v>
+      </c>
+      <c r="E10" t="s">
         <v>20</v>
       </c>
-      <c r="B7" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C7" t="s">
+      <c r="F10" s="1" t="s">
         <v>21</v>
       </c>
-      <c r="D7" s="1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4">
-      <c r="A8" t="s">
-        <v>20</v>
-      </c>
-      <c r="B8" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C8" t="s">
-        <v>24</v>
-      </c>
-      <c r="D8" s="1" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4">
-      <c r="A9" t="s">
-        <v>20</v>
-      </c>
-      <c r="B9" s="5" t="s">
-        <v>5</v>
-      </c>
-      <c r="C9" t="s">
-        <v>6</v>
-      </c>
-      <c r="D9" s="1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4">
-      <c r="A10" t="s">
-        <v>26</v>
-      </c>
-      <c r="B10" s="5" t="s">
-        <v>27</v>
-      </c>
-      <c r="C10" t="s">
-        <v>28</v>
-      </c>
-      <c r="D10" s="1" t="s">
-        <v>29</v>
+      <c r="G10" t="s">
+        <v>50</v>
+      </c>
+      <c r="H10" t="s">
+        <v>51</v>
       </c>
     </row>
   </sheetData>

</xml_diff>